<commit_message>
Final model tweaks for 458.A3
</commit_message>
<xml_diff>
--- a/458 - Artificial Intelligence & Deep Learning/458.7 - Natural Language Processing: RNN, LTSM, 1D CNN/experiment_results.xlsx
+++ b/458 - Artificial Intelligence & Deep Learning/458.7 - Natural Language Processing: RNN, LTSM, 1D CNN/experiment_results.xlsx
@@ -626,35 +626,35 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4284778535366058</v>
+        <v>0.4558551907539368</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8528508543968201</v>
+        <v>0.8417368531227112</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4612316191196442</v>
+        <v>0.4799478054046631</v>
       </c>
       <c r="G5" t="n">
-        <v>0.8389999866485596</v>
+        <v>0.8231666684150696</v>
       </c>
       <c r="H5" t="n">
-        <v>0.8405263157894737</v>
+        <v>0.8394736842105263</v>
       </c>
       <c r="I5" t="n">
-        <v>0.8405263157894737</v>
+        <v>0.8394736842105263</v>
       </c>
       <c r="J5" t="n">
-        <v>0.8405263157894737</v>
+        <v>0.8394736842105263</v>
       </c>
       <c r="K5" t="n">
-        <v>0.8405263157894737</v>
+        <v>0.8394736842105263</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>18:20</t>
+          <t>7:27</t>
         </is>
       </c>
     </row>
@@ -752,35 +752,35 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3253275454044342</v>
+        <v>0.3552636504173279</v>
       </c>
       <c r="E8" t="n">
-        <v>0.8888245820999146</v>
+        <v>0.8744210600852966</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4610510170459747</v>
+        <v>0.397102952003479</v>
       </c>
       <c r="G8" t="n">
-        <v>0.8603333234786987</v>
+        <v>0.8615000247955322</v>
       </c>
       <c r="H8" t="n">
-        <v>0.8682894736842105</v>
+        <v>0.8597368421052631</v>
       </c>
       <c r="I8" t="n">
-        <v>0.8682894736842105</v>
+        <v>0.8597368421052631</v>
       </c>
       <c r="J8" t="n">
-        <v>0.8682894736842105</v>
+        <v>0.8597368421052631</v>
       </c>
       <c r="K8" t="n">
-        <v>0.8682894736842105</v>
+        <v>0.8597368421052631</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>16:55</t>
+          <t>14:38</t>
         </is>
       </c>
     </row>

</xml_diff>